<commit_message>
Modelado ML - Tablas finales
</commit_message>
<xml_diff>
--- a/4_Modelado/Recursos/Sintetico.xlsx
+++ b/4_Modelado/Recursos/Sintetico.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Split mensual" sheetId="1" r:id="rId1"/>
@@ -25,73 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="47">
-  <si>
-    <t>producto</t>
-  </si>
-  <si>
-    <t>periodo</t>
-  </si>
-  <si>
-    <t>tipo_clasificador</t>
-  </si>
-  <si>
-    <t>clasificador</t>
-  </si>
-  <si>
-    <t>tipo_evaluacion</t>
-  </si>
-  <si>
-    <t>PACI</t>
-  </si>
-  <si>
-    <t>KSTA</t>
-  </si>
-  <si>
-    <t>Nada_PREC</t>
-  </si>
-  <si>
-    <t>Nada_RCALL</t>
-  </si>
-  <si>
-    <t>Nada_FMEA</t>
-  </si>
-  <si>
-    <t>Nada_ROCA</t>
-  </si>
-  <si>
-    <t>Nada_PRCA</t>
-  </si>
-  <si>
-    <t>Medio_PREC</t>
-  </si>
-  <si>
-    <t>Medio_RCALL</t>
-  </si>
-  <si>
-    <t>Medio_FMEA</t>
-  </si>
-  <si>
-    <t>Medio_ROCA</t>
-  </si>
-  <si>
-    <t>Medio_PRCA</t>
-  </si>
-  <si>
-    <t>Mucho_PREC</t>
-  </si>
-  <si>
-    <t>Mucho_RCALL</t>
-  </si>
-  <si>
-    <t>Mucho_FMEA</t>
-  </si>
-  <si>
-    <t>Mucho_ROCA</t>
-  </si>
-  <si>
-    <t>Mucho_PRCA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="62">
   <si>
     <t>MENSUAL</t>
   </si>
@@ -167,6 +101,150 @@
   <si>
     <t>crossEstratificado</t>
   </si>
+  <si>
+    <t>PROD.</t>
+  </si>
+  <si>
+    <t>PERIODO</t>
+  </si>
+  <si>
+    <t>CLASIFICADOR</t>
+  </si>
+  <si>
+    <t>KAPPA</t>
+  </si>
+  <si>
+    <t>Nada - 
+RCALL</t>
+  </si>
+  <si>
+    <t>Nada - 
+FMEA</t>
+  </si>
+  <si>
+    <t>Nada - 
+ROCA</t>
+  </si>
+  <si>
+    <t>Nada - 
+PRCA</t>
+  </si>
+  <si>
+    <t>Medio - 
+PREC</t>
+  </si>
+  <si>
+    <t>Nada - 
+PREC</t>
+  </si>
+  <si>
+    <t>Medio - 
+RCALL</t>
+  </si>
+  <si>
+    <t>Medio - 
+FMEA</t>
+  </si>
+  <si>
+    <t>Medio - 
+ROCA</t>
+  </si>
+  <si>
+    <t>Medio - 
+PRCA</t>
+  </si>
+  <si>
+    <t>Mucho - 
+PREC</t>
+  </si>
+  <si>
+    <t>Mucho - 
+RCALL</t>
+  </si>
+  <si>
+    <t>Mucho - 
+FMEA</t>
+  </si>
+  <si>
+    <t>Mucho - 
+ROCA</t>
+  </si>
+  <si>
+    <t>Mucho - 
+PRCA</t>
+  </si>
+  <si>
+    <t>TIPO
+EVAL.</t>
+  </si>
+  <si>
+    <t>TIPO
+CLASIF.</t>
+  </si>
+  <si>
+    <t>PORC.
+ACIER.</t>
+  </si>
+  <si>
+    <t>Nada -
+PREC</t>
+  </si>
+  <si>
+    <t>Nada -
+RCALL</t>
+  </si>
+  <si>
+    <t>Nada -
+FMEA</t>
+  </si>
+  <si>
+    <t>Nada -
+ROCA</t>
+  </si>
+  <si>
+    <t>Nada -
+PRCA</t>
+  </si>
+  <si>
+    <t>Medio -
+PREC</t>
+  </si>
+  <si>
+    <t>Medio -
+RCALL</t>
+  </si>
+  <si>
+    <t>Medio -
+FMEA</t>
+  </si>
+  <si>
+    <t>Medio -
+ROCA</t>
+  </si>
+  <si>
+    <t>Medio -
+PRCA</t>
+  </si>
+  <si>
+    <t>Mucho -
+PREC</t>
+  </si>
+  <si>
+    <t>Mucho -
+RCALL</t>
+  </si>
+  <si>
+    <t>Mucho -
+FMEA</t>
+  </si>
+  <si>
+    <t>Mucho -
+ROCA</t>
+  </si>
+  <si>
+    <t>Mucho -
+PRCA</t>
+  </si>
 </sst>
 </file>
 
@@ -181,7 +259,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -207,9 +285,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -222,7 +306,35 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -235,7 +347,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -248,7 +360,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -261,7 +373,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -274,7 +386,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -287,7 +399,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -300,7 +412,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -313,7 +425,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -326,7 +438,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -339,7 +451,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -352,7 +464,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -365,7 +477,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -378,7 +490,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -391,7 +503,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -404,7 +516,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -417,7 +529,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -430,7 +542,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -443,7 +555,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -456,7 +568,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -469,7 +581,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -482,7 +594,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -495,7 +607,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -508,7 +620,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -521,7 +633,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -534,7 +646,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -547,7 +659,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -560,7 +672,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -573,7 +685,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -586,7 +698,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -599,7 +711,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -612,7 +724,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -625,7 +737,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -638,7 +750,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -651,7 +763,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -664,7 +776,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -677,7 +789,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -690,7 +802,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -703,7 +815,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -716,7 +828,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -729,7 +841,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -742,7 +854,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -755,7 +867,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -768,7 +880,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -781,7 +893,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -794,7 +906,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -807,7 +919,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -820,33 +932,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -866,7 +952,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:V37" headerRowDxfId="26" dataDxfId="24" totalsRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:V37" headerRowDxfId="1" dataDxfId="25" totalsRowDxfId="26">
   <autoFilter ref="A1:V37">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -892,35 +978,35 @@
     <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="22">
-    <tableColumn id="1" name="producto" totalsRowLabel="Total" dataDxfId="48"/>
-    <tableColumn id="2" name="periodo" dataDxfId="47"/>
-    <tableColumn id="3" name="tipo_clasificador" dataDxfId="46"/>
-    <tableColumn id="4" name="clasificador" dataDxfId="45"/>
-    <tableColumn id="5" name="tipo_evaluacion" dataDxfId="44"/>
-    <tableColumn id="6" name="PACI" dataDxfId="43"/>
-    <tableColumn id="7" name="KSTA" dataDxfId="42"/>
-    <tableColumn id="8" name="Nada_PREC" dataDxfId="41"/>
-    <tableColumn id="9" name="Nada_RCALL" dataDxfId="40"/>
-    <tableColumn id="10" name="Nada_FMEA" dataDxfId="39"/>
-    <tableColumn id="11" name="Nada_ROCA" dataDxfId="38"/>
-    <tableColumn id="12" name="Nada_PRCA" dataDxfId="37"/>
-    <tableColumn id="13" name="Medio_PREC" dataDxfId="36"/>
-    <tableColumn id="14" name="Medio_RCALL" dataDxfId="35"/>
-    <tableColumn id="15" name="Medio_FMEA" dataDxfId="34"/>
-    <tableColumn id="16" name="Medio_ROCA" dataDxfId="33"/>
-    <tableColumn id="17" name="Medio_PRCA" dataDxfId="32"/>
-    <tableColumn id="18" name="Mucho_PREC" dataDxfId="31"/>
-    <tableColumn id="19" name="Mucho_RCALL" dataDxfId="30"/>
-    <tableColumn id="20" name="Mucho_FMEA" dataDxfId="29"/>
-    <tableColumn id="21" name="Mucho_ROCA" dataDxfId="28"/>
-    <tableColumn id="22" name="Mucho_PRCA" totalsRowFunction="sum" dataDxfId="27"/>
+    <tableColumn id="1" name="PROD." totalsRowLabel="Total" dataDxfId="48"/>
+    <tableColumn id="2" name="PERIODO" dataDxfId="47"/>
+    <tableColumn id="3" name="TIPO_x000a_CLASIF." dataDxfId="46"/>
+    <tableColumn id="4" name="CLASIFICADOR" dataDxfId="45"/>
+    <tableColumn id="5" name="TIPO_x000a_EVAL." dataDxfId="44"/>
+    <tableColumn id="6" name="PORC._x000a_ACIER." dataDxfId="43"/>
+    <tableColumn id="7" name="KAPPA" dataDxfId="42"/>
+    <tableColumn id="8" name="Nada - _x000a_PREC" dataDxfId="41"/>
+    <tableColumn id="9" name="Nada - _x000a_RCALL" dataDxfId="40"/>
+    <tableColumn id="10" name="Nada - _x000a_FMEA" dataDxfId="39"/>
+    <tableColumn id="11" name="Nada - _x000a_ROCA" dataDxfId="38"/>
+    <tableColumn id="12" name="Nada - _x000a_PRCA" dataDxfId="37"/>
+    <tableColumn id="13" name="Medio - _x000a_PREC" dataDxfId="36"/>
+    <tableColumn id="14" name="Medio - _x000a_RCALL" dataDxfId="35"/>
+    <tableColumn id="15" name="Medio - _x000a_FMEA" dataDxfId="34"/>
+    <tableColumn id="16" name="Medio - _x000a_ROCA" dataDxfId="33"/>
+    <tableColumn id="17" name="Medio - _x000a_PRCA" dataDxfId="32"/>
+    <tableColumn id="18" name="Mucho - _x000a_PREC" dataDxfId="31"/>
+    <tableColumn id="19" name="Mucho - _x000a_RCALL" dataDxfId="30"/>
+    <tableColumn id="20" name="Mucho - _x000a_FMEA" dataDxfId="29"/>
+    <tableColumn id="21" name="Mucho - _x000a_ROCA" dataDxfId="28"/>
+    <tableColumn id="22" name="Mucho - _x000a_PRCA" totalsRowFunction="sum" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:V37" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:V37" totalsRowShown="0" headerRowDxfId="0" dataDxfId="2">
   <autoFilter ref="A1:V37">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -946,28 +1032,28 @@
     <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="22">
-    <tableColumn id="1" name="producto" dataDxfId="23"/>
-    <tableColumn id="2" name="periodo" dataDxfId="22"/>
-    <tableColumn id="3" name="tipo_clasificador" dataDxfId="21"/>
-    <tableColumn id="4" name="clasificador" dataDxfId="20"/>
-    <tableColumn id="5" name="tipo_evaluacion" dataDxfId="19"/>
-    <tableColumn id="6" name="PACI" dataDxfId="18"/>
-    <tableColumn id="7" name="KSTA" dataDxfId="17"/>
-    <tableColumn id="8" name="Nada_PREC" dataDxfId="16"/>
-    <tableColumn id="9" name="Nada_RCALL" dataDxfId="15"/>
-    <tableColumn id="10" name="Nada_FMEA" dataDxfId="14"/>
-    <tableColumn id="11" name="Nada_ROCA" dataDxfId="13"/>
-    <tableColumn id="12" name="Nada_PRCA" dataDxfId="12"/>
-    <tableColumn id="13" name="Medio_PREC" dataDxfId="11"/>
-    <tableColumn id="14" name="Medio_RCALL" dataDxfId="10"/>
-    <tableColumn id="15" name="Medio_FMEA" dataDxfId="9"/>
-    <tableColumn id="16" name="Medio_ROCA" dataDxfId="8"/>
-    <tableColumn id="17" name="Medio_PRCA" dataDxfId="7"/>
-    <tableColumn id="18" name="Mucho_PREC" dataDxfId="6"/>
-    <tableColumn id="19" name="Mucho_RCALL" dataDxfId="5"/>
-    <tableColumn id="20" name="Mucho_FMEA" dataDxfId="4"/>
-    <tableColumn id="21" name="Mucho_ROCA" dataDxfId="3"/>
-    <tableColumn id="22" name="Mucho_PRCA" dataDxfId="2"/>
+    <tableColumn id="1" name="PROD." dataDxfId="24"/>
+    <tableColumn id="2" name="PERIODO" dataDxfId="23"/>
+    <tableColumn id="3" name="TIPO_x000a_CLASIF." dataDxfId="22"/>
+    <tableColumn id="4" name="CLASIFICADOR" dataDxfId="21"/>
+    <tableColumn id="5" name="TIPO_x000a_EVAL." dataDxfId="20"/>
+    <tableColumn id="6" name="PORC._x000a_ACIER." dataDxfId="19"/>
+    <tableColumn id="7" name="KAPPA" dataDxfId="18"/>
+    <tableColumn id="8" name="Nada -_x000a_PREC" dataDxfId="17"/>
+    <tableColumn id="9" name="Nada -_x000a_RCALL" dataDxfId="16"/>
+    <tableColumn id="10" name="Nada -_x000a_FMEA" dataDxfId="15"/>
+    <tableColumn id="11" name="Nada -_x000a_ROCA" dataDxfId="14"/>
+    <tableColumn id="12" name="Nada -_x000a_PRCA" dataDxfId="13"/>
+    <tableColumn id="13" name="Medio -_x000a_PREC" dataDxfId="12"/>
+    <tableColumn id="14" name="Medio -_x000a_RCALL" dataDxfId="11"/>
+    <tableColumn id="15" name="Medio -_x000a_FMEA" dataDxfId="10"/>
+    <tableColumn id="16" name="Medio -_x000a_ROCA" dataDxfId="9"/>
+    <tableColumn id="17" name="Medio -_x000a_PRCA" dataDxfId="8"/>
+    <tableColumn id="18" name="Mucho -_x000a_PREC" dataDxfId="7"/>
+    <tableColumn id="19" name="Mucho -_x000a_RCALL" dataDxfId="6"/>
+    <tableColumn id="20" name="Mucho -_x000a_FMEA" dataDxfId="5"/>
+    <tableColumn id="21" name="Mucho -_x000a_ROCA" dataDxfId="4"/>
+    <tableColumn id="22" name="Mucho -_x000a_PRCA" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1238,97 +1324,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="1"/>
-    <col min="8" max="8" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="1" customWidth="1"/>
-    <col min="10" max="11" width="13.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="14.85546875" style="1" customWidth="1"/>
-    <col min="17" max="18" width="14.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" style="1" customWidth="1"/>
-    <col min="20" max="21" width="15.140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
+    <row r="1" spans="1:22" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -1336,16 +1418,16 @@
         <v>100</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
         <v>57.14</v>
@@ -1404,16 +1486,16 @@
         <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1">
         <v>42.86</v>
@@ -1472,16 +1554,16 @@
         <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1">
         <v>42.86</v>
@@ -1540,16 +1622,16 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1">
         <v>57.14</v>
@@ -1608,16 +1690,16 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1">
         <v>50</v>
@@ -1676,16 +1758,16 @@
         <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1">
         <v>71.430000000000007</v>
@@ -1744,16 +1826,16 @@
         <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1">
         <v>57.14</v>
@@ -1812,16 +1894,16 @@
         <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F9" s="1">
         <v>57.14</v>
@@ -1880,16 +1962,16 @@
         <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1">
         <v>57.14</v>
@@ -1948,16 +2030,16 @@
         <v>100</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1">
         <v>57.14</v>
@@ -2016,16 +2098,16 @@
         <v>100</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1">
         <v>42.86</v>
@@ -2084,16 +2166,16 @@
         <v>100</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1">
         <v>57.14</v>
@@ -2152,16 +2234,16 @@
         <v>100</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1">
         <v>57.14</v>
@@ -2220,16 +2302,16 @@
         <v>100</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1">
         <v>42.86</v>
@@ -2288,16 +2370,16 @@
         <v>100</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1">
         <v>71.430000000000007</v>
@@ -2356,16 +2438,16 @@
         <v>100</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1">
         <v>64.290000000000006</v>
@@ -2424,16 +2506,16 @@
         <v>100</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1">
         <v>50</v>
@@ -2492,16 +2574,16 @@
         <v>100</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F19" s="1">
         <v>42.86</v>
@@ -2560,16 +2642,16 @@
         <v>106</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1">
         <v>57.14</v>
@@ -2628,16 +2710,16 @@
         <v>106</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F21" s="1">
         <v>57.14</v>
@@ -2696,16 +2778,16 @@
         <v>106</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F22" s="1">
         <v>57.14</v>
@@ -2764,16 +2846,16 @@
         <v>106</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F23" s="1">
         <v>50</v>
@@ -2832,16 +2914,16 @@
         <v>106</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F24" s="1">
         <v>64.290000000000006</v>
@@ -2900,16 +2982,16 @@
         <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F25" s="1">
         <v>71.430000000000007</v>
@@ -2968,16 +3050,16 @@
         <v>106</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1">
         <v>71.430000000000007</v>
@@ -3036,16 +3118,16 @@
         <v>106</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F27" s="1">
         <v>71.430000000000007</v>
@@ -3104,16 +3186,16 @@
         <v>106</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F28" s="1">
         <v>71.430000000000007</v>
@@ -3172,16 +3254,16 @@
         <v>106</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F29" s="1">
         <v>78.569999999999993</v>
@@ -3240,16 +3322,16 @@
         <v>106</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F30" s="1">
         <v>57.14</v>
@@ -3308,16 +3390,16 @@
         <v>106</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F31" s="1">
         <v>64.290000000000006</v>
@@ -3376,16 +3458,16 @@
         <v>106</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F32" s="1">
         <v>57.14</v>
@@ -3444,16 +3526,16 @@
         <v>106</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F33" s="1">
         <v>71.430000000000007</v>
@@ -3512,16 +3594,16 @@
         <v>106</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F34" s="1">
         <v>71.430000000000007</v>
@@ -3580,16 +3662,16 @@
         <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F35" s="1">
         <v>78.569999999999993</v>
@@ -3648,16 +3730,16 @@
         <v>106</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F36" s="1">
         <v>71.430000000000007</v>
@@ -3716,16 +3798,16 @@
         <v>106</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F37" s="1">
         <v>64.290000000000006</v>
@@ -3792,97 +3874,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="1"/>
-    <col min="8" max="8" width="13.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="1" customWidth="1"/>
-    <col min="10" max="11" width="13.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="14.85546875" style="1" customWidth="1"/>
-    <col min="17" max="18" width="14.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" style="1" customWidth="1"/>
-    <col min="20" max="21" width="15.140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="7.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
+    <row r="1" spans="1:22" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -3890,16 +3968,16 @@
         <v>100</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="1">
         <v>58.82</v>
@@ -3958,16 +4036,16 @@
         <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1">
         <v>52.94</v>
@@ -4026,16 +4104,16 @@
         <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1">
         <v>52.94</v>
@@ -4094,16 +4172,16 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1">
         <v>64.709999999999994</v>
@@ -4162,16 +4240,16 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1">
         <v>55.88</v>
@@ -4230,16 +4308,16 @@
         <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1">
         <v>76.47</v>
@@ -4298,16 +4376,16 @@
         <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1">
         <v>55.88</v>
@@ -4366,16 +4444,16 @@
         <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1">
         <v>70.59</v>
@@ -4434,16 +4512,16 @@
         <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1">
         <v>52.94</v>
@@ -4502,16 +4580,16 @@
         <v>100</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1">
         <v>70.59</v>
@@ -4570,16 +4648,16 @@
         <v>100</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1">
         <v>64.709999999999994</v>
@@ -4638,16 +4716,16 @@
         <v>100</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1">
         <v>58.82</v>
@@ -4706,16 +4784,16 @@
         <v>100</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1">
         <v>55.88</v>
@@ -4774,16 +4852,16 @@
         <v>100</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1">
         <v>61.76</v>
@@ -4842,16 +4920,16 @@
         <v>100</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1">
         <v>76.47</v>
@@ -4910,16 +4988,16 @@
         <v>100</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1">
         <v>73.53</v>
@@ -4978,16 +5056,16 @@
         <v>100</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F18" s="1">
         <v>64.709999999999994</v>
@@ -5046,16 +5124,16 @@
         <v>100</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1">
         <v>61.76</v>
@@ -5114,16 +5192,16 @@
         <v>106</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F20" s="1">
         <v>79.41</v>
@@ -5182,16 +5260,16 @@
         <v>106</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1">
         <v>73.53</v>
@@ -5250,16 +5328,16 @@
         <v>106</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1">
         <v>73.53</v>
@@ -5318,16 +5396,16 @@
         <v>106</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1">
         <v>67.650000000000006</v>
@@ -5386,16 +5464,16 @@
         <v>106</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1">
         <v>70.59</v>
@@ -5454,16 +5532,16 @@
         <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F25" s="1">
         <v>73.53</v>
@@ -5522,16 +5600,16 @@
         <v>106</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F26" s="1">
         <v>73.53</v>
@@ -5590,16 +5668,16 @@
         <v>106</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1">
         <v>82.35</v>
@@ -5658,16 +5736,16 @@
         <v>106</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F28" s="1">
         <v>79.41</v>
@@ -5726,16 +5804,16 @@
         <v>106</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F29" s="1">
         <v>79.41</v>
@@ -5794,16 +5872,16 @@
         <v>106</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F30" s="1">
         <v>73.53</v>
@@ -5862,16 +5940,16 @@
         <v>106</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F31" s="1">
         <v>64.709999999999994</v>
@@ -5930,16 +6008,16 @@
         <v>106</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F32" s="1">
         <v>82.35</v>
@@ -5998,16 +6076,16 @@
         <v>106</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F33" s="1">
         <v>70.59</v>
@@ -6066,16 +6144,16 @@
         <v>106</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F34" s="1">
         <v>73.53</v>
@@ -6134,16 +6212,16 @@
         <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F35" s="1">
         <v>73.53</v>
@@ -6202,16 +6280,16 @@
         <v>106</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F36" s="1">
         <v>82.35</v>
@@ -6270,16 +6348,16 @@
         <v>106</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F37" s="1">
         <v>73.53</v>

</xml_diff>